<commit_message>
Update morning 26th april, slight change in the direction of the study paper ~  more directly about developing effects for PA (also more data in the database)
</commit_message>
<xml_diff>
--- a/List of papers providing effect size benchmarks.xlsx
+++ b/List of papers providing effect size benchmarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Dissertation Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Effect Size paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0138081F-B0C9-4CD8-BF7A-402229E8B208}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE90FF8-EB1A-40F1-AC60-A09B58BABE32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19190" windowHeight="6170" xr2:uid="{68B35B6A-722E-4416-95E4-0DF7A301094D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>Cooper, H., &amp; Findley, M. (1982). Expected Effect Sizes: Estimates for Statistical Power Analysis in Social Psychology</t>
   </si>
@@ -93,9 +93,6 @@
     <t>75th percentile</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>unit of analysis (article or test)</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Empirically Derived Guidelines for Interpreting Effect Size in Social Psychology Andrey Lovakov Elena Agadullina https://psyarxiv.com/2epc4/</t>
   </si>
   <si>
-    <t>Effect size guidelines for individual differences researchers Author links open overlay panel Gilles E.GignacEva T.Szodorai</t>
-  </si>
-  <si>
     <t xml:space="preserve">The five topics that appeared most frequeently in nine social psychology textbooks were determined: altruism, aggression, attitude change, attraction and conformaty…. Two chapters covering each topic were randomly chosen, and an attempt was made to retrieve the reserach cited in each chapter. ... Only one measure of effect size was retrieved from each report. The sentence in the textbook that referred to the article's hypothesis appeared in a report, or if the comment in the textbook were ambiguous, the test was used that best matched the textbook's description. </t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Bosco et al. (2015)</t>
   </si>
   <si>
-    <t>Articles reported in social psychology textbooks reporting d (2t/(sqrt(df error)))</t>
-  </si>
-  <si>
     <t>Articles reported in social psychology textbooks reporting f (df = 1)</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>Articles reported in social psychology textbooks reporting r</t>
   </si>
   <si>
-    <t>Articles reported in social psychology textbooks reporting w (df = 1) (sqrt(chisquare/n))</t>
-  </si>
-  <si>
     <t>See the article for effect sizes by content area</t>
   </si>
   <si>
@@ -204,24 +192,9 @@
     <t>Effect sizes from meta-analyses of Heart Rate Variability Studies</t>
   </si>
   <si>
-    <t>Effect sizes from meta-analyses published in the top 30 impact factor management journals</t>
-  </si>
-  <si>
     <t>We sampled 18 journals frequently cited in cognitive neuroscience and psychology. Our aim was to collect data on the latest publication practices. To this end, we analyzed 4 y of regular issues for all journals published between Jan 2011 to Aug 2014</t>
   </si>
   <si>
-    <t>Psychiatry</t>
-  </si>
-  <si>
-    <t>Cognitive neuroscience</t>
-  </si>
-  <si>
-    <t>Psychology</t>
-  </si>
-  <si>
-    <t>All fields</t>
-  </si>
-  <si>
     <t>Nature Neuroscience, Neuron, Brain, The Journal of Neuroscience, Cerebral Cortex, NeuroImage, Cortex, Biological Psychology, Neuropsychologia, Neuroscience</t>
   </si>
   <si>
@@ -238,6 +211,54 @@
   </si>
   <si>
     <t>We searched PsycLIT and other computerized databases for references to meta-analysis, examined a number of special journal issues and books on metaanalysis (e.g., Miller &amp; Cooper, 1991), used the Social Sciences Citation Index to locate documents that had cited certain key references on meta-analysis (e.g., Rosenthal, 1984), consulted lists of meta-analyses that had been compiled by others (e.g., Bausell, Li, Gau, &amp; Soeken, 1995), and manually scanned all of the issues of certain journals (e.g., Psychological Bulletin). ...</t>
+  </si>
+  <si>
+    <t>Articles reported in social psychology textbooks reporting d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Articles reported in social psychology textbooks reporting w (df = 1) </t>
+  </si>
+  <si>
+    <t>Effect sizes from meta-analyses published in the top 30 impact factor management journals before 2012</t>
+  </si>
+  <si>
+    <t>Cognitive neuroscience, psychology, psychiatry articles published in high impact journals, 2011 - 2014</t>
+  </si>
+  <si>
+    <t>Cognitive neuroscience articles published in high impact journals, 2011 - 2014</t>
+  </si>
+  <si>
+    <t>Psychology articles published in high impact journals, 2011 - 2014</t>
+  </si>
+  <si>
+    <t>Psychiatry articles published in high impact journals, 2011 - 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social psychology articles, </t>
+  </si>
+  <si>
+    <t>n (number of units of analysis included)</t>
+  </si>
+  <si>
+    <t>(33912 effects from literature - not necessarily independent)</t>
+  </si>
+  <si>
+    <t>Hemphill, J. F. (2003). Interpreting the magnitudes of correlation coefficients. American Psychologist, 58(1), 78–80.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ... Meta-analyses were excluded if the results were reported as Cohen's d, odds-ratios, inter-rater reliability coefficients, intra-class correlations, or heritability coefficients. Additionally, meta-analyses that were based on longitudinal designs (i.e., correlations between the same measures across time) and consensual validity type coefficients (correlations between the same measures as assessed by different people) were also excluded. Thus, only meta-analyses which were relevant to the association between two conceptually distinct constructs were included in the investigation. Based on the application of the exclusion criteria, a total of 87 meta-analyses remained in the sample … . A total of 708 observed correlations were derived from the sample of 87 meta-analyses (8.13 correlations per meta-analysis). Additionally, a total of 345 true score correlations were derived from 24 of the meta-analyses that included at least one correlation disattenuated for imperfect reliability.2 For the purposes of the analyses, all of the negative correlations were transformed into absolute correlations, as it would be inappropriate to calculate measures of central tendency on a combination of negative and positive values, in this case.</t>
+  </si>
+  <si>
+    <t>Meta-analyses of correlational studies published in leading personality journals - Personality and Individual Differences, Psychological Bulletin, Journal of Research in Personality, Journal of Personality and Social Psychology, Journal of Personality, and Intelligence (no time frame provided)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gignac &amp; Szodorai (2016) Effect size guidelines for individual differences researchers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from Gignac &amp; Szodorai (2016) Effect size guidelines for individual differences researchers </t>
+  </si>
+  <si>
+    <t>Note: "Observed correlations" recorded here (see table 1 of Gignac and Szodorai), although corrected true score correlations are also reported in the article</t>
   </si>
 </sst>
 </file>
@@ -278,13 +299,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA576A4-F028-4F47-9BB3-C41347066A5F}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="91" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -618,13 +640,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
@@ -648,7 +670,7 @@
         <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -659,13 +681,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1">
         <v>701</v>
@@ -694,13 +716,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>14</v>
@@ -715,7 +737,7 @@
         <v>0.62</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -726,13 +748,13 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>113</v>
@@ -747,7 +769,7 @@
         <v>0.3</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -758,13 +780,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>72</v>
@@ -779,7 +801,7 @@
         <v>0.54</v>
       </c>
       <c r="L5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -790,13 +812,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E6">
         <v>23</v>
@@ -811,7 +833,7 @@
         <v>0.22</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
@@ -822,13 +844,13 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -843,7 +865,7 @@
         <v>0.16</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
         <v>14</v>
@@ -854,16 +876,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8">
         <v>0.22700000000000001</v>
@@ -875,13 +897,13 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -889,13 +911,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>26841</v>
@@ -910,13 +932,13 @@
         <v>0.65400000000000003</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
       </c>
       <c r="N9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -924,13 +946,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>7888</v>
@@ -945,13 +967,13 @@
         <v>1.22</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -959,13 +981,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>16887</v>
@@ -980,13 +1002,13 @@
         <v>0.96</v>
       </c>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
       </c>
       <c r="N11" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -994,13 +1016,13 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>2066</v>
@@ -1015,21 +1037,45 @@
         <v>0.91</v>
       </c>
       <c r="L12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
       </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" t="s">
-        <v>70</v>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13">
+        <v>474</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13">
+        <v>0.21</v>
+      </c>
+      <c r="J13">
+        <v>0.18</v>
+      </c>
+      <c r="K13">
+        <v>0.15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>27</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -1040,17 +1086,20 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E14">
         <v>297</v>
       </c>
+      <c r="F14">
+        <v>293</v>
+      </c>
       <c r="G14">
         <v>0.26</v>
       </c>
@@ -1061,21 +1110,45 @@
         <v>0.51</v>
       </c>
       <c r="L14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
       </c>
       <c r="N14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>0.11</v>
+      </c>
+      <c r="H15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J15">
+        <v>0.19</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1091,42 +1164,50 @@
         <v>15</v>
       </c>
       <c r="M17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
         <v>36</v>
-      </c>
-      <c r="M19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N21" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="M22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:1">

</xml_diff>

<commit_message>
Adding a few more papers to database, minor edits to effect size measures.docx
</commit_message>
<xml_diff>
--- a/List of papers providing effect size benchmarks.xlsx
+++ b/List of papers providing effect size benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Effect Size paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE90FF8-EB1A-40F1-AC60-A09B58BABE32}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C548299-820A-421C-A650-24765A7551D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19190" windowHeight="6170" xr2:uid="{68B35B6A-722E-4416-95E4-0DF7A301094D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>Cooper, H., &amp; Findley, M. (1982). Expected Effect Sizes: Estimates for Statistical Power Analysis in Social Psychology</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>Note: "Observed correlations" recorded here (see table 1 of Gignac and Szodorai), although corrected true score correlations are also reported in the article</t>
+  </si>
+  <si>
+    <t>87 meta-analyses (708 observed correlations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Scholar "average effect size" (also, looking at his data, meta-anlyses = 297 effects from 293 studies, only 4 fewer) </t>
+  </si>
+  <si>
+    <t>Hyde, J (1981) How large are cognitive gender differences? A meta-analysis using !w² and d.</t>
   </si>
 </sst>
 </file>
@@ -623,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA576A4-F028-4F47-9BB3-C41347066A5F}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="91" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -1113,7 +1122,7 @@
         <v>26</v>
       </c>
       <c r="M14" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="N14" t="s">
         <v>44</v>
@@ -1132,6 +1141,9 @@
       <c r="D15" t="s">
         <v>50</v>
       </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
       <c r="G15">
         <v>0.11</v>
       </c>
@@ -1208,6 +1220,11 @@
       </c>
       <c r="M22" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:1">

</xml_diff>

<commit_message>
Breaking effect size measure paper into Approaches to formal sample size determination and an effect size measures paper - the effect size measures paper has information about the actual effect size measures, the other has information about when to take a min clincical sig effect approach or estimate an effect. I also updated some of the info in the database of empirical effect size benchmarks.
</commit_message>
<xml_diff>
--- a/List of papers providing effect size benchmarks.xlsx
+++ b/List of papers providing effect size benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Effect Size paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C548299-820A-421C-A650-24765A7551D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37DEB05-F59A-40E1-A39F-D422C0495C89}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19190" windowHeight="6170" xr2:uid="{68B35B6A-722E-4416-95E4-0DF7A301094D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="97">
   <si>
     <t>Cooper, H., &amp; Findley, M. (1982). Expected Effect Sizes: Estimates for Statistical Power Analysis in Social Psychology</t>
   </si>
@@ -99,9 +99,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>Empirically Derived Guidelines for Interpreting Effect Size in Social Psychology Andrey Lovakov Elena Agadullina https://psyarxiv.com/2epc4/</t>
-  </si>
-  <si>
     <t xml:space="preserve">The five topics that appeared most frequeently in nine social psychology textbooks were determined: altruism, aggression, attitude change, attraction and conformaty…. Two chapters covering each topic were randomly chosen, and an attempt was made to retrieve the reserach cited in each chapter. ... Only one measure of effect size was retrieved from each report. The sentence in the textbook that referred to the article's hypothesis appeared in a report, or if the comment in the textbook were ambiguous, the test was used that best matched the textbook's description. </t>
   </si>
   <si>
@@ -129,27 +126,15 @@
     <t>Articles for inclusion in our review were identified by examining the contents of journals that appeared on the list of Eigenfactor.org’s top 30 most impactful management journals and had published at least one meta-analysis by June 1, 2012. We then used Academic Search Premier to search these journals for articles whose titles included the terms meta-analysis, meta-analyses, meta-analytic, or quantitative review. This search yielded 350 articles appearing in eleven journals: Academy of Management Journal, Human Performance, Journal of Applied Psychology, Journal of Management, Journal of Management Studies, Journal of Occupational and Organizational Psychology, Journal of Organizational Behavior, Organizational Behavior and Human Decision Processes, Organization Studies, Personnel Psychology, and The Leadership Quarterly.</t>
   </si>
   <si>
-    <t>Visible learning a synthesis of over 800 meta-analyses relating to achievement / John A.C. Hattie.</t>
-  </si>
-  <si>
     <t>Grey literature search</t>
   </si>
   <si>
-    <t>Found from https://www.psychometrica.de/effect_size.html</t>
-  </si>
-  <si>
     <t>776 "conclusions" from  258 meta-analyses</t>
   </si>
   <si>
-    <t>Mazen (1987)</t>
-  </si>
-  <si>
     <t>From Paterson, T. A., Harms, P. D., Steel, P., &amp; Credé, M. (2015). An Assessment of the Magnitude of Effect Sizes: Evidence From 30 Years of Meta-Analysis in Management</t>
   </si>
   <si>
-    <t>Bosco et al. (2015)</t>
-  </si>
-  <si>
     <t>Articles reported in social psychology textbooks reporting f (df = 1)</t>
   </si>
   <si>
@@ -249,32 +234,95 @@
     <t xml:space="preserve"> ... Meta-analyses were excluded if the results were reported as Cohen's d, odds-ratios, inter-rater reliability coefficients, intra-class correlations, or heritability coefficients. Additionally, meta-analyses that were based on longitudinal designs (i.e., correlations between the same measures across time) and consensual validity type coefficients (correlations between the same measures as assessed by different people) were also excluded. Thus, only meta-analyses which were relevant to the association between two conceptually distinct constructs were included in the investigation. Based on the application of the exclusion criteria, a total of 87 meta-analyses remained in the sample … . A total of 708 observed correlations were derived from the sample of 87 meta-analyses (8.13 correlations per meta-analysis). Additionally, a total of 345 true score correlations were derived from 24 of the meta-analyses that included at least one correlation disattenuated for imperfect reliability.2 For the purposes of the analyses, all of the negative correlations were transformed into absolute correlations, as it would be inappropriate to calculate measures of central tendency on a combination of negative and positive values, in this case.</t>
   </si>
   <si>
-    <t>Meta-analyses of correlational studies published in leading personality journals - Personality and Individual Differences, Psychological Bulletin, Journal of Research in Personality, Journal of Personality and Social Psychology, Journal of Personality, and Intelligence (no time frame provided)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gignac &amp; Szodorai (2016) Effect size guidelines for individual differences researchers </t>
   </si>
   <si>
-    <t xml:space="preserve">from Gignac &amp; Szodorai (2016) Effect size guidelines for individual differences researchers </t>
-  </si>
-  <si>
     <t>Note: "Observed correlations" recorded here (see table 1 of Gignac and Szodorai), although corrected true score correlations are also reported in the article</t>
   </si>
   <si>
-    <t>87 meta-analyses (708 observed correlations)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Google Scholar "average effect size" (also, looking at his data, meta-anlyses = 297 effects from 293 studies, only 4 fewer) </t>
   </si>
   <si>
-    <t>Hyde, J (1981) How large are cognitive gender differences? A meta-analysis using !w² and d.</t>
+    <t>Glass' d</t>
+  </si>
+  <si>
+    <t>Standard search procedures were used to identify 1,000 documents: Psychological Abstracts, Dissertation Abstracts, and branching off of bibliographies of the documents themselves. Of those documents located, approximately 500 were selected for inclusion in the study, and 375 were fully analyzed. To be selected, a study had to have at least one therapy treatment group compared to an untreated group or to a different therapy group. The rigor of the research design was not a selection criterion but was one of several features of the individual study to be related to the effect of the treatment in that study. The definition of psychotherapy used to select the studies was presented by Meltzoff and Kornreich (1970)</t>
+  </si>
+  <si>
+    <t>Studies of psychotherapy with a non-treatment control group published before 1977</t>
+  </si>
+  <si>
+    <t>effect size</t>
+  </si>
+  <si>
+    <t>Meta-analyses of correlational studies published in leading personality journals - Personality and Individual Differences, Psychological Bulletin, Journal of Research in Personality, Journal of Personality and Social Psychology, Journal of Personality, and Intelligence, 1985-2015</t>
+  </si>
+  <si>
+    <t>Hattie (2009) Visible learning a synthesis of over 800 meta-analyses relating to achievement</t>
+  </si>
+  <si>
+    <t>"It was possible to locate a total of about 800 meta-analyses, which encompassed 52,637 studies, and provided 146,142 eﬀect sizes about the inﬂuence of some program, policy, or innovation on academic achievement in school (early childhood, elementary, high, and tertiary). Topics not included are those concerning English as a second language, aﬀective or physical outcomes, and meta-analyses where the number of studies was fewer than four. When the same meta-analysis has been published multiple times, (e.g., when dissertations are rewritten as articles), only the most recent or most accessible is included. As can be imagined, these eﬀects cover most school subjects (although the majority are reading, mathematics, science, and social studies), all ages, and a myriad of comparisons. These eﬀects are based on many millions of students across the main areas of inﬂuence—from the student, the home, the eﬀects of schools, teachers, curricula, and teaching methods and strategies. The total number of students identifed in the meta-analyses is large. Only 286 of the meta-analyses included total sample size but together these alone totaled 83 million students. Using the average sample size per study, this would multiply out to about 236 million students in total. However, it is likely that many students would have participated in more than one study, and thus this is a gross estimate of sample size. Even so, it would be safe to conclude that these studies are based on many millions of students"</t>
+  </si>
+  <si>
+    <t>Meta-anaylses of educational interventions</t>
+  </si>
+  <si>
+    <t>d (unclear which standardiser)</t>
+  </si>
+  <si>
+    <t>Area of research</t>
+  </si>
+  <si>
+    <t>Clinical psychology</t>
+  </si>
+  <si>
+    <t>Social psychology</t>
+  </si>
+  <si>
+    <t>Note: effect size from articles cited in introductory textbooks, presumably inflated / not generalisable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note - uses glass' delta - the SD of the control group is the standardiser </t>
+  </si>
+  <si>
+    <t>Cognitive neuroscience, psychology and psychiatry</t>
+  </si>
+  <si>
+    <t>Cognitive neuroscience</t>
+  </si>
+  <si>
+    <t>Psychology</t>
+  </si>
+  <si>
+    <t>Psychiatry</t>
+  </si>
+  <si>
+    <t>Andrey &amp; Agadullina  (2018, pre-print) Empirically Derived Guidelines for Interpreting Effect Size in Social https://psyarxiv.com/2epc4/</t>
+  </si>
+  <si>
+    <t>Bosco et al. (2015) Correlational effect size benchmarks</t>
+  </si>
+  <si>
+    <t>Hear rate variability studies</t>
+  </si>
+  <si>
+    <t>Personality and Social psychology</t>
+  </si>
+  <si>
+    <t>Clinicial psychology</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +334,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="MinionPro-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242021"/>
+      <name val="BemboStd"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -316,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,605 +694,723 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA576A4-F028-4F47-9BB3-C41347066A5F}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
+  <cols>
+    <col min="1" max="2" width="8.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>70</v>
-      </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>701</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.26819999999999999</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.15890000000000001</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
       </c>
       <c r="F3">
         <v>14</v>
       </c>
-      <c r="I3">
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="J3">
         <v>1.19</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.62</v>
       </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
       <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4">
-        <v>113</v>
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
       </c>
       <c r="F4">
         <v>113</v>
       </c>
-      <c r="I4">
+      <c r="G4">
+        <v>113</v>
+      </c>
+      <c r="J4">
         <v>0.45</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.3</v>
       </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
       <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5">
-        <v>72</v>
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
       </c>
       <c r="F5">
         <v>72</v>
       </c>
-      <c r="I5">
+      <c r="G5">
+        <v>72</v>
+      </c>
+      <c r="J5">
         <v>0.6</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.54</v>
       </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
       <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>23</v>
       </c>
       <c r="F6">
         <v>23</v>
       </c>
-      <c r="I6">
+      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="J6">
         <v>0.48</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.22</v>
       </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
       <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
       </c>
       <c r="F7">
         <v>15</v>
       </c>
-      <c r="I7">
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="J7">
         <v>0.26</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.16</v>
       </c>
-      <c r="L7" t="s">
-        <v>32</v>
-      </c>
       <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>64</v>
-      </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8">
         <v>0.22700000000000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.2</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.13500000000000001</v>
       </c>
-      <c r="L8" t="s">
-        <v>27</v>
-      </c>
       <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
         <v>14</v>
       </c>
-      <c r="N8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>26841</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3801</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.93799999999999994</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.65400000000000003</v>
       </c>
-      <c r="L9" t="s">
-        <v>26</v>
-      </c>
       <c r="M9" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" t="s">
         <v>14</v>
       </c>
-      <c r="N9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>7888</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1192</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.34</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1.22</v>
       </c>
-      <c r="L10" t="s">
-        <v>26</v>
-      </c>
       <c r="M10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" t="s">
         <v>14</v>
       </c>
-      <c r="N10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>16887</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2261</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.96</v>
       </c>
-      <c r="L11" t="s">
-        <v>26</v>
-      </c>
       <c r="M11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" t="s">
         <v>14</v>
       </c>
-      <c r="N11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2066</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>348</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.23</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.91</v>
       </c>
-      <c r="L12" t="s">
-        <v>26</v>
-      </c>
       <c r="M12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" t="s">
         <v>14</v>
       </c>
-      <c r="N12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13">
         <v>474</v>
       </c>
-      <c r="F13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13">
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13">
         <v>0.21</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.18</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0.15</v>
       </c>
-      <c r="L13" t="s">
-        <v>27</v>
-      </c>
       <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
         <v>297</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>293</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.26</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.88</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.51</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>708</v>
+      </c>
+      <c r="H15">
+        <v>0.11</v>
+      </c>
+      <c r="I15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K15">
+        <v>0.19</v>
+      </c>
+      <c r="M15" t="s">
         <v>26</v>
       </c>
-      <c r="M14" t="s">
-        <v>79</v>
-      </c>
-      <c r="N14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15">
-        <v>0.11</v>
-      </c>
-      <c r="H15">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="J15">
-        <v>0.19</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>14</v>
       </c>
-      <c r="N15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>12</v>
       </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <v>833</v>
+      </c>
+      <c r="G16">
+        <v>375</v>
+      </c>
+      <c r="J16">
+        <v>0.68</v>
+      </c>
+      <c r="L16">
+        <v>0.67</v>
+      </c>
       <c r="M16" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" t="s">
+      <c r="O16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="B17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <v>816</v>
+      </c>
+      <c r="G19">
+        <v>52649</v>
+      </c>
+      <c r="J19">
+        <v>0.4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="M20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" t="s">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
       </c>
       <c r="N21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="M22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating approaches to formal sample size determination.docx - minor changes + adding figures
</commit_message>
<xml_diff>
--- a/List of papers providing effect size benchmarks.xlsx
+++ b/List of papers providing effect size benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsingletonthorn\Documents\PhD\Effect Size paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37DEB05-F59A-40E1-A39F-D422C0495C89}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8B0AB5-C135-49C7-9D56-712C91395F15}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19190" windowHeight="6170" xr2:uid="{68B35B6A-722E-4416-95E4-0DF7A301094D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="100">
   <si>
     <t>Cooper, H., &amp; Findley, M. (1982). Expected Effect Sizes: Estimates for Statistical Power Analysis in Social Psychology</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/cdev.13079</t>
+  </si>
+  <si>
+    <t>Bergmann, C., Tsuji, S., Piccinini Page, E., Lewis Molly, L., Braginsky, M., Frank Michael, C., &amp; Cristia, A. (2018). Promoting Replicability in Developmental Research Through Meta‐analyses- Insights From Lan</t>
+  </si>
+  <si>
+    <t>Twitter - https://twitter.com/chbergma/status/993739362180452352</t>
   </si>
 </sst>
 </file>
@@ -696,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA576A4-F028-4F47-9BB3-C41347066A5F}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="68" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -1405,8 +1414,15 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="N22" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2"/>

</xml_diff>